<commit_message>
parsing 5 yaml files
</commit_message>
<xml_diff>
--- a/cmake-build-debug/excel_file.xlsx
+++ b/cmake-build-debug/excel_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>tache3</t>
+  </si>
+  <si>
+    <t>site4</t>
+  </si>
+  <si>
+    <t>tache4</t>
+  </si>
+  <si>
+    <t>site5</t>
+  </si>
+  <si>
+    <t>tache5</t>
   </si>
 </sst>
 </file>
@@ -385,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,6 +462,34 @@
         <v>120</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2">
+        <v>44618</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2">
+        <v>44618</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>